<commit_message>
Final firmware version and made some new logs
</commit_message>
<xml_diff>
--- a/Temperature Logger/Logs/2023-10-02_18-26-00_temperature.xlsx
+++ b/Temperature Logger/Logs/2023-10-02_18-26-00_temperature.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uapt33090-my.sharepoint.com/personal/joaolmf_ua_pt/Documents/UNI/DPE/GitHug_Mk4/Leapfrog_Creatr_Mk4/Temperature Logger/Logs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_B46F472DAB4190164CFE31D2F8F2D3C2B4505887" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01EEFFB9-7734-4317-9D38-CBCBF6FAFF1F}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2895" yWindow="2865" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -25,8 +31,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +95,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -133,7 +147,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -167,6 +181,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -201,9 +216,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -376,14 +392,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -391,15 +413,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.203306</v>
+        <v>0.20330599999999999</v>
       </c>
       <c r="B2">
         <v>26.93</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.406757</v>
       </c>
@@ -407,63 +429,63 @@
         <v>27.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2.610656</v>
+        <v>2.6106560000000001</v>
       </c>
       <c r="B4">
         <v>27.05</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3.814167</v>
+        <v>3.8141669999999999</v>
       </c>
       <c r="B5">
         <v>27.27</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5.024474</v>
+        <v>5.0244739999999997</v>
       </c>
       <c r="B6">
         <v>27.84</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6.227254</v>
+        <v>6.2272540000000003</v>
       </c>
       <c r="B7">
         <v>28.41</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7.42998</v>
+        <v>7.4299799999999996</v>
       </c>
       <c r="B8">
         <v>29.32</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8.635809</v>
+        <v>8.6358090000000001</v>
       </c>
       <c r="B9">
         <v>30.73</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9.840468</v>
+        <v>9.8404679999999995</v>
       </c>
       <c r="B10">
         <v>32.08</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11.044248</v>
       </c>
@@ -471,23 +493,23 @@
         <v>33.85</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>12.246949</v>
+        <v>12.246949000000001</v>
       </c>
       <c r="B12">
         <v>35.67</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>13.452611</v>
+        <v>13.452610999999999</v>
       </c>
       <c r="B13">
         <v>37.42</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14.656649</v>
       </c>
@@ -495,7 +517,7 @@
         <v>39.58</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15.858558</v>
       </c>
@@ -503,15 +525,15 @@
         <v>41.76</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>17.062191</v>
+        <v>17.062190999999999</v>
       </c>
       <c r="B16">
         <v>44.12</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>18.266375</v>
       </c>
@@ -519,7 +541,7 @@
         <v>46.51</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>19.470506</v>
       </c>
@@ -527,15 +549,15 @@
         <v>49.08</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>20.672826</v>
+        <v>20.672826000000001</v>
       </c>
       <c r="B19">
         <v>51.65</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>21.876234</v>
       </c>
@@ -543,23 +565,23 @@
         <v>54.26</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>23.081183</v>
+        <v>23.081182999999999</v>
       </c>
       <c r="B21">
         <v>56.93</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>24.285493</v>
+        <v>24.285492999999999</v>
       </c>
       <c r="B22">
         <v>59.74</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>25.489601</v>
       </c>
@@ -567,39 +589,39 @@
         <v>62.41</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>26.692268</v>
+        <v>26.692267999999999</v>
       </c>
       <c r="B24">
-        <v>65.26000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>65.260000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>27.8969</v>
+        <v>27.896899999999999</v>
       </c>
       <c r="B25">
         <v>67.97</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>29.100643</v>
+        <v>29.100643000000002</v>
       </c>
       <c r="B26">
-        <v>70.84999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>70.849999999999994</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>30.302904</v>
+        <v>30.302904000000002</v>
       </c>
       <c r="B27">
         <v>73.59</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>31.506909</v>
       </c>
@@ -607,111 +629,111 @@
         <v>76.44</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>32.711633</v>
+        <v>32.711632999999999</v>
       </c>
       <c r="B29">
         <v>79.36</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>33.91571</v>
+        <v>33.915709999999997</v>
       </c>
       <c r="B30">
-        <v>82.18000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>82.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>35.121817</v>
       </c>
       <c r="B31">
-        <v>84.95999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>84.96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>36.323683</v>
+        <v>36.323683000000003</v>
       </c>
       <c r="B32">
-        <v>87.73999999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>87.74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>37.528564</v>
+        <v>37.528564000000003</v>
       </c>
       <c r="B33">
         <v>90.44</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>38.730598</v>
+        <v>38.730598000000001</v>
       </c>
       <c r="B34">
         <v>93.28</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>39.935283</v>
+        <v>39.935282999999998</v>
       </c>
       <c r="B35">
         <v>96.05</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>41.139625</v>
+        <v>41.139625000000002</v>
       </c>
       <c r="B36">
         <v>98.89</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>42.342473</v>
+        <v>42.342472999999998</v>
       </c>
       <c r="B37">
         <v>101.61</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>43.54966</v>
+        <v>43.549660000000003</v>
       </c>
       <c r="B38">
         <v>104.31</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>44.751944</v>
+        <v>44.751944000000002</v>
       </c>
       <c r="B39">
         <v>106.93</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>45.956611</v>
+        <v>45.956611000000002</v>
       </c>
       <c r="B40">
         <v>109.66</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>47.160504</v>
+        <v>47.160504000000003</v>
       </c>
       <c r="B41">
         <v>112.33</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>48.364314</v>
       </c>
@@ -719,15 +741,15 @@
         <v>114.93</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>49.566163</v>
+        <v>49.566163000000003</v>
       </c>
       <c r="B43">
         <v>117.54</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>50.769624</v>
       </c>
@@ -735,335 +757,335 @@
         <v>120.07</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>51.973688</v>
+        <v>51.973688000000003</v>
       </c>
       <c r="B45">
         <v>122.68</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>53.182601</v>
+        <v>53.182600999999998</v>
       </c>
       <c r="B46">
         <v>125.2</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>54.385722</v>
+        <v>54.385722000000001</v>
       </c>
       <c r="B47">
         <v>127.85</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>55.590455</v>
+        <v>55.590454999999999</v>
       </c>
       <c r="B48">
         <v>130.28</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>56.793089</v>
+        <v>56.793089000000002</v>
       </c>
       <c r="B49">
-        <v>132.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>132.69999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>57.995857</v>
+        <v>57.995857000000001</v>
       </c>
       <c r="B50">
         <v>135.04</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>59.20098</v>
+        <v>59.200980000000001</v>
       </c>
       <c r="B51">
         <v>137.5</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>60.405801</v>
+        <v>60.405800999999997</v>
       </c>
       <c r="B52">
         <v>139.91</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>61.609519</v>
+        <v>61.609518999999999</v>
       </c>
       <c r="B53">
         <v>142.31</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>62.812219</v>
+        <v>62.812218999999999</v>
       </c>
       <c r="B54">
         <v>144.63</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>64.016372</v>
+        <v>64.016372000000004</v>
       </c>
       <c r="B55">
-        <v>146.95</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>146.94999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>65.221907</v>
+        <v>65.221907000000002</v>
       </c>
       <c r="B56">
-        <v>149.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>149.30000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>66.42707</v>
+        <v>66.427070000000001</v>
       </c>
       <c r="B57">
         <v>151.68</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>67.63087</v>
+        <v>67.630870000000002</v>
       </c>
       <c r="B58">
         <v>153.97</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>68.835244</v>
+        <v>68.835244000000003</v>
       </c>
       <c r="B59">
         <v>156.19</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>70.037294</v>
+        <v>70.037294000000003</v>
       </c>
       <c r="B60">
-        <v>158.45</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>158.44999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>71.264976</v>
+        <v>71.264976000000004</v>
       </c>
       <c r="B61">
         <v>160.72</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>72.46884300000001</v>
+        <v>72.468843000000007</v>
       </c>
       <c r="B62">
         <v>163.09</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>73.673953</v>
+        <v>73.673952999999997</v>
       </c>
       <c r="B63">
         <v>165.21</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>74.87827299999999</v>
+        <v>74.878272999999993</v>
       </c>
       <c r="B64">
         <v>167.5</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>76.081996</v>
+        <v>76.081996000000004</v>
       </c>
       <c r="B65">
         <v>169.79</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>77.286574</v>
+        <v>77.286574000000002</v>
       </c>
       <c r="B66">
         <v>172.11</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>78.48956800000001</v>
+        <v>78.489568000000006</v>
       </c>
       <c r="B67">
         <v>174.22</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>79.696178</v>
+        <v>79.696178000000003</v>
       </c>
       <c r="B68">
         <v>176.42</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>80.902041</v>
+        <v>80.902040999999997</v>
       </c>
       <c r="B69">
         <v>178.58</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>82.104209</v>
+        <v>82.104208999999997</v>
       </c>
       <c r="B70">
         <v>180.67</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>83.30863600000001</v>
+        <v>83.308636000000007</v>
       </c>
       <c r="B71">
         <v>182.79</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>84.51321</v>
+        <v>84.513210000000001</v>
       </c>
       <c r="B72">
         <v>185</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>85.71819499999999</v>
+        <v>85.718194999999994</v>
       </c>
       <c r="B73">
         <v>187.19</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>86.923061</v>
+        <v>86.923061000000004</v>
       </c>
       <c r="B74">
         <v>189.48</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>88.124959</v>
+        <v>88.124959000000004</v>
       </c>
       <c r="B75">
         <v>191.7</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>89.328165</v>
+        <v>89.328164999999998</v>
       </c>
       <c r="B76">
         <v>193.98</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>90.533295</v>
+        <v>90.533294999999995</v>
       </c>
       <c r="B77">
         <v>195.91</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>91.73638099999999</v>
+        <v>91.736380999999994</v>
       </c>
       <c r="B78">
         <v>197.84</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>92.94052600000001</v>
+        <v>92.940526000000006</v>
       </c>
       <c r="B79">
         <v>199.66</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>94.14386500000001</v>
+        <v>94.143865000000005</v>
       </c>
       <c r="B80">
         <v>201.53</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>95.349683</v>
+        <v>95.349682999999999</v>
       </c>
       <c r="B81">
         <v>203.47</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>96.552425</v>
+        <v>96.552424999999999</v>
       </c>
       <c r="B82">
         <v>205.47</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>97.75573199999999</v>
+        <v>97.755731999999995</v>
       </c>
       <c r="B83">
         <v>207.66</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>98.96673</v>
+        <v>98.966729999999998</v>
       </c>
       <c r="B84">
         <v>209.53</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>100.170696</v>
+        <v>100.17069600000001</v>
       </c>
       <c r="B85">
         <v>211.72</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>101.3734</v>
       </c>
@@ -1071,15 +1093,15 @@
         <v>213.59</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>102.578184</v>
+        <v>102.57818399999999</v>
       </c>
       <c r="B87">
         <v>215.42</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>103.783736</v>
       </c>
@@ -1087,23 +1109,23 @@
         <v>217.29</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>104.985301</v>
+        <v>104.98530100000001</v>
       </c>
       <c r="B89">
         <v>219.58</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>106.188916</v>
+        <v>106.18891600000001</v>
       </c>
       <c r="B90">
         <v>221.43</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>107.391098</v>
       </c>
@@ -1111,23 +1133,23 @@
         <v>223.04</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>108.597052</v>
+        <v>108.59705200000001</v>
       </c>
       <c r="B92">
         <v>224.46</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>109.803283</v>
+        <v>109.80328299999999</v>
       </c>
       <c r="B93">
         <v>226.5</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>111.004651</v>
       </c>
@@ -1135,15 +1157,15 @@
         <v>228.75</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>112.207136</v>
+        <v>112.20713600000001</v>
       </c>
       <c r="B95">
         <v>230.75</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>113.410393</v>
       </c>
@@ -1151,7 +1173,7 @@
         <v>232.75</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>114.614199</v>
       </c>
@@ -1159,7 +1181,7 @@
         <v>234.25</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>115.820544</v>
       </c>
@@ -1167,15 +1189,15 @@
         <v>236</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>117.024425</v>
+        <v>117.02442499999999</v>
       </c>
       <c r="B99">
         <v>237.75</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>118.228674</v>
       </c>
@@ -1183,7 +1205,7 @@
         <v>239.5</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>119.433066</v>
       </c>
@@ -1191,7 +1213,7 @@
         <v>241.25</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>120.636438</v>
       </c>
@@ -1199,15 +1221,15 @@
         <v>243.12</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>121.841422</v>
+        <v>121.84142199999999</v>
       </c>
       <c r="B103">
         <v>244.69</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>123.047499</v>
       </c>
@@ -1215,23 +1237,23 @@
         <v>245.94</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>124.252739</v>
+        <v>124.25273900000001</v>
       </c>
       <c r="B105">
         <v>246.87</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>125.454907</v>
+        <v>125.45490700000001</v>
       </c>
       <c r="B106">
         <v>247.81</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>126.65693</v>
       </c>
@@ -1239,7 +1261,7 @@
         <v>248.12</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>127.859341</v>
       </c>
@@ -1247,15 +1269,15 @@
         <v>248.44</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>129.062723</v>
+        <v>129.06272300000001</v>
       </c>
       <c r="B109">
         <v>248.75</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>130.266402</v>
       </c>
@@ -1263,23 +1285,23 @@
         <v>248.12</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>131.469724</v>
+        <v>131.46972400000001</v>
       </c>
       <c r="B111">
         <v>248.12</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>132.675227</v>
+        <v>132.67522700000001</v>
       </c>
       <c r="B112">
         <v>248.12</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>133.877914</v>
       </c>
@@ -1287,15 +1309,15 @@
         <v>248.12</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>135.081854</v>
+        <v>135.08185399999999</v>
       </c>
       <c r="B114">
         <v>247.81</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>136.285135</v>
       </c>
@@ -1303,7 +1325,7 @@
         <v>247.81</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>137.508274</v>
       </c>
@@ -1311,7 +1333,7 @@
         <v>247.5</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>138.710928</v>
       </c>
@@ -1319,7 +1341,7 @@
         <v>247.19</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>139.914556</v>
       </c>
@@ -1327,7 +1349,7 @@
         <v>246.87</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>141.118538</v>
       </c>
@@ -1335,15 +1357,15 @@
         <v>246.56</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>142.322503</v>
+        <v>142.32250300000001</v>
       </c>
       <c r="B120">
         <v>246.56</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>143.526197</v>
       </c>
@@ -1351,71 +1373,71 @@
         <v>246.25</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>144.730251</v>
+        <v>144.73025100000001</v>
       </c>
       <c r="B122">
         <v>246.25</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>145.933566</v>
+        <v>145.93356600000001</v>
       </c>
       <c r="B123">
         <v>246.25</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>147.137266</v>
+        <v>147.13726600000001</v>
       </c>
       <c r="B124">
         <v>245.94</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>148.340292</v>
+        <v>148.34029200000001</v>
       </c>
       <c r="B125">
         <v>245.94</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>149.545054</v>
+        <v>149.54505399999999</v>
       </c>
       <c r="B126">
         <v>245.94</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>150.748769</v>
+        <v>150.74876900000001</v>
       </c>
       <c r="B127">
         <v>246.25</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>151.952087</v>
+        <v>151.95208700000001</v>
       </c>
       <c r="B128">
         <v>246.25</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>153.160632</v>
+        <v>153.16063199999999</v>
       </c>
       <c r="B129">
         <v>246.25</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>154.365522</v>
       </c>
@@ -1423,7 +1445,7 @@
         <v>246.25</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>155.568296</v>
       </c>
@@ -1431,23 +1453,23 @@
         <v>246.25</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>156.772928</v>
+        <v>156.77292800000001</v>
       </c>
       <c r="B132">
         <v>246.56</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>157.97607</v>
+        <v>157.97606999999999</v>
       </c>
       <c r="B133">
         <v>246.56</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>159.181253</v>
       </c>
@@ -1455,7 +1477,7 @@
         <v>246.87</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>160.388631</v>
       </c>
@@ -1463,7 +1485,7 @@
         <v>247.19</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>161.592826</v>
       </c>
@@ -1471,15 +1493,15 @@
         <v>247.19</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>162.797633</v>
+        <v>162.79763299999999</v>
       </c>
       <c r="B137">
         <v>247.81</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>164.002994</v>
       </c>
@@ -1487,39 +1509,39 @@
         <v>247.81</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>165.204527</v>
+        <v>165.20452700000001</v>
       </c>
       <c r="B139">
         <v>248.12</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>166.408764</v>
+        <v>166.40876399999999</v>
       </c>
       <c r="B140">
         <v>247.81</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>167.612463</v>
+        <v>167.61246299999999</v>
       </c>
       <c r="B141">
         <v>248.12</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>168.816746</v>
+        <v>168.81674599999999</v>
       </c>
       <c r="B142">
         <v>248.44</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>170.021433</v>
       </c>
@@ -1527,15 +1549,15 @@
         <v>248.75</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>171.228366</v>
+        <v>171.22836599999999</v>
       </c>
       <c r="B144">
         <v>249.06</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>172.43069</v>
       </c>
@@ -1543,31 +1565,31 @@
         <v>249.37</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>173.634605</v>
+        <v>173.63460499999999</v>
       </c>
       <c r="B146">
         <v>249.37</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>174.838399</v>
+        <v>174.83839900000001</v>
       </c>
       <c r="B147">
         <v>249.69</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>176.041058</v>
+        <v>176.04105799999999</v>
       </c>
       <c r="B148">
         <v>250</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>177.247412</v>
       </c>
@@ -1575,15 +1597,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>178.450397</v>
+        <v>178.45039700000001</v>
       </c>
       <c r="B150">
         <v>249.69</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>179.654492</v>
       </c>
@@ -1591,7 +1613,7 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>180.859407</v>
       </c>
@@ -1599,15 +1621,15 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>182.062699</v>
+        <v>182.06269900000001</v>
       </c>
       <c r="B153">
         <v>249.69</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>183.265548</v>
       </c>
@@ -1615,39 +1637,39 @@
         <v>250</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>184.475253</v>
+        <v>184.47525300000001</v>
       </c>
       <c r="B155">
         <v>250</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>185.677339</v>
+        <v>185.67733899999999</v>
       </c>
       <c r="B156">
         <v>250</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>186.881397</v>
+        <v>186.88139699999999</v>
       </c>
       <c r="B157">
         <v>250</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>188.087618</v>
+        <v>188.08761799999999</v>
       </c>
       <c r="B158">
         <v>250</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>189.29065</v>
       </c>
@@ -1655,31 +1677,31 @@
         <v>250</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>190.494423</v>
+        <v>190.49442300000001</v>
       </c>
       <c r="B160">
         <v>250.62</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>191.698805</v>
+        <v>191.69880499999999</v>
       </c>
       <c r="B161">
         <v>250.31</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>192.903068</v>
+        <v>192.90306799999999</v>
       </c>
       <c r="B162">
         <v>250.62</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>194.104872</v>
       </c>
@@ -1687,7 +1709,7 @@
         <v>250.62</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>195.30703</v>
       </c>
@@ -1695,7 +1717,7 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>196.512216</v>
       </c>
@@ -1703,23 +1725,23 @@
         <v>250.62</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>197.71663</v>
+        <v>197.71663000000001</v>
       </c>
       <c r="B166">
         <v>250.62</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>198.920855</v>
+        <v>198.92085499999999</v>
       </c>
       <c r="B167">
         <v>250.31</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>200.124798</v>
       </c>
@@ -1727,7 +1749,7 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>201.329442</v>
       </c>
@@ -1735,7 +1757,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>202.532951</v>
       </c>
@@ -1743,7 +1765,7 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>203.73612</v>
       </c>
@@ -1751,7 +1773,7 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>204.939615</v>
       </c>
@@ -1759,7 +1781,7 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>206.14337</v>
       </c>
@@ -1767,23 +1789,23 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>207.349656</v>
+        <v>207.34965600000001</v>
       </c>
       <c r="B174">
         <v>250.31</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>208.55386</v>
+        <v>208.55385999999999</v>
       </c>
       <c r="B175">
         <v>250.31</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>209.759109</v>
       </c>
@@ -1791,7 +1813,7 @@
         <v>250.62</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>210.96408</v>
       </c>
@@ -1799,15 +1821,15 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>212.167794</v>
+        <v>212.16779399999999</v>
       </c>
       <c r="B178">
         <v>250</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>213.369765</v>
       </c>
@@ -1815,15 +1837,15 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>214.573147</v>
+        <v>214.57314700000001</v>
       </c>
       <c r="B180">
         <v>249.69</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>215.777773</v>
       </c>
@@ -1831,15 +1853,15 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>216.983535</v>
+        <v>216.98353499999999</v>
       </c>
       <c r="B182">
         <v>249.69</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>218.187094</v>
       </c>
@@ -1847,31 +1869,31 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>219.390067</v>
+        <v>219.39006699999999</v>
       </c>
       <c r="B184">
         <v>249.69</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>220.594433</v>
+        <v>220.59443300000001</v>
       </c>
       <c r="B185">
         <v>249.69</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>221.798951</v>
+        <v>221.79895099999999</v>
       </c>
       <c r="B186">
         <v>250</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>223.00124</v>
       </c>
@@ -1879,7 +1901,7 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>224.204926</v>
       </c>
@@ -1887,15 +1909,15 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>225.408497</v>
+        <v>225.40849700000001</v>
       </c>
       <c r="B189">
         <v>249.37</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>226.612402</v>
       </c>
@@ -1903,7 +1925,7 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>227.81858</v>
       </c>
@@ -1911,15 +1933,15 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>229.022294</v>
+        <v>229.02229399999999</v>
       </c>
       <c r="B192">
         <v>250</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>230.227868</v>
       </c>
@@ -1927,15 +1949,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>231.431054</v>
+        <v>231.43105399999999</v>
       </c>
       <c r="B194">
         <v>250.31</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>232.635456</v>
       </c>
@@ -1943,15 +1965,15 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>233.840247</v>
+        <v>233.84024700000001</v>
       </c>
       <c r="B196">
         <v>250</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>235.043789</v>
       </c>
@@ -1959,47 +1981,47 @@
         <v>250</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>236.249241</v>
+        <v>236.24924100000001</v>
       </c>
       <c r="B198">
         <v>250</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>237.451002</v>
+        <v>237.45100199999999</v>
       </c>
       <c r="B199">
         <v>250</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>238.656985</v>
+        <v>238.65698499999999</v>
       </c>
       <c r="B200">
         <v>250.31</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>239.860892</v>
+        <v>239.86089200000001</v>
       </c>
       <c r="B201">
         <v>250</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>241.063001</v>
+        <v>241.06300100000001</v>
       </c>
       <c r="B202">
         <v>250</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>242.266538</v>
       </c>
@@ -2007,7 +2029,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>243.470426</v>
       </c>
@@ -2015,15 +2037,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>244.675978</v>
+        <v>244.67597799999999</v>
       </c>
       <c r="B205">
         <v>250</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>245.879031</v>
       </c>
@@ -2031,7 +2053,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>247.083099</v>
       </c>
@@ -2039,31 +2061,31 @@
         <v>250</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>248.288301</v>
+        <v>248.28830099999999</v>
       </c>
       <c r="B208">
         <v>250</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>249.499739</v>
+        <v>249.49973900000001</v>
       </c>
       <c r="B209">
         <v>250</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>250.702399</v>
+        <v>250.70239900000001</v>
       </c>
       <c r="B210">
         <v>250</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>251.906845</v>
       </c>
@@ -2071,7 +2093,7 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>253.111919</v>
       </c>
@@ -2079,23 +2101,23 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>254.315847</v>
+        <v>254.31584699999999</v>
       </c>
       <c r="B213">
         <v>249.69</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>255.518188</v>
+        <v>255.51818800000001</v>
       </c>
       <c r="B214">
         <v>250</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>256.720482</v>
       </c>
@@ -2103,39 +2125,39 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>257.922715</v>
+        <v>257.92271499999998</v>
       </c>
       <c r="B216">
         <v>250</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>259.12773</v>
+        <v>259.12772999999999</v>
       </c>
       <c r="B217">
         <v>250.31</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>260.331198</v>
+        <v>260.33119799999997</v>
       </c>
       <c r="B218">
         <v>250</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>261.537384</v>
+        <v>261.53738399999997</v>
       </c>
       <c r="B219">
         <v>250.31</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>262.742884</v>
       </c>
@@ -2143,7 +2165,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>263.947565</v>
       </c>
@@ -2151,23 +2173,23 @@
         <v>250</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>265.151674</v>
+        <v>265.15167400000001</v>
       </c>
       <c r="B222">
         <v>249.69</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>266.35532</v>
+        <v>266.35532000000001</v>
       </c>
       <c r="B223">
         <v>249.37</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>267.56054</v>
       </c>
@@ -2175,31 +2197,31 @@
         <v>249.37</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>268.762304</v>
+        <v>268.76230399999997</v>
       </c>
       <c r="B225">
         <v>249.06</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>269.965996</v>
+        <v>269.96599600000002</v>
       </c>
       <c r="B226">
         <v>249.37</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>271.169235</v>
+        <v>271.16923500000001</v>
       </c>
       <c r="B227">
         <v>249.69</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>272.37446</v>
       </c>
@@ -2207,15 +2229,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>273.576929</v>
+        <v>273.57692900000001</v>
       </c>
       <c r="B229">
         <v>250</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>274.781046</v>
       </c>
@@ -2223,7 +2245,7 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>275.985026</v>
       </c>
@@ -2231,23 +2253,23 @@
         <v>250.62</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>277.189329</v>
+        <v>277.18932899999999</v>
       </c>
       <c r="B232">
         <v>250.62</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>278.393071</v>
+        <v>278.39307100000002</v>
       </c>
       <c r="B233">
         <v>250.62</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>279.595822</v>
       </c>
@@ -2255,23 +2277,23 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>280.802247</v>
+        <v>280.80224700000002</v>
       </c>
       <c r="B235">
         <v>250.31</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>282.007132</v>
+        <v>282.00713200000001</v>
       </c>
       <c r="B236">
         <v>249.69</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>283.211206</v>
       </c>
@@ -2279,15 +2301,15 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>284.415677</v>
+        <v>284.41567700000002</v>
       </c>
       <c r="B238">
         <v>249.69</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>285.632744</v>
       </c>
@@ -2295,39 +2317,39 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240">
-        <v>286.837892</v>
+        <v>286.83789200000001</v>
       </c>
       <c r="B240">
         <v>249.69</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241">
-        <v>288.041008</v>
+        <v>288.04100799999998</v>
       </c>
       <c r="B241">
         <v>249.69</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242">
-        <v>289.247619</v>
+        <v>289.24761899999999</v>
       </c>
       <c r="B242">
         <v>250.31</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243">
-        <v>290.450135</v>
+        <v>290.45013499999999</v>
       </c>
       <c r="B243">
         <v>250.62</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>291.654582</v>
       </c>
@@ -2335,39 +2357,39 @@
         <v>250.31</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>292.859549</v>
+        <v>292.85954900000002</v>
       </c>
       <c r="B245">
         <v>250.62</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>294.063792</v>
+        <v>294.06379199999998</v>
       </c>
       <c r="B246">
         <v>250.31</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>295.275729</v>
+        <v>295.27572900000001</v>
       </c>
       <c r="B247">
         <v>250.31</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248">
-        <v>296.478709</v>
+        <v>296.47870899999998</v>
       </c>
       <c r="B248">
         <v>250</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>297.681622</v>
       </c>
@@ -2375,17 +2397,17 @@
         <v>250</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250">
-        <v>298.886137</v>
+        <v>298.88613700000002</v>
       </c>
       <c r="B250">
         <v>249.69</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251">
-        <v>300.09047</v>
+        <v>300.09046999999998</v>
       </c>
       <c r="B251">
         <v>249.06</v>

</xml_diff>